<commit_message>
updated excel with final revisions to part 2 title and abstract
</commit_message>
<xml_diff>
--- a/Part_2_data/false_match_on_title.xlsx
+++ b/Part_2_data/false_match_on_title.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/Part_2_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF37E0-7370-1440-B039-51FD9DA27FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D441C5B-7F5D-4E44-BBCC-2D71B0058903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="1100" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34180" yWindow="1100" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$324</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="33" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="881">
   <si>
     <t>DOI</t>
   </si>
@@ -2678,10 +2678,28 @@
     <t>Count of error_classification</t>
   </si>
   <si>
-    <t>Error or noise classification</t>
-  </si>
-  <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Information gain</t>
+  </si>
+  <si>
+    <t>information gain</t>
+  </si>
+  <si>
+    <t>information loss</t>
+  </si>
+  <si>
+    <t>total full set</t>
+  </si>
+  <si>
+    <t>Error and noise classification</t>
+  </si>
+  <si>
+    <t>Percentage of non-matching</t>
+  </si>
+  <si>
+    <t>Percentage of whole set</t>
   </si>
 </sst>
 </file>
@@ -2760,26 +2778,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2793,7 +2830,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Poppy Riddle" refreshedDate="45989.50280115741" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="324" xr:uid="{BE8D97D8-8858-4E4F-B159-AD67E1A7AF2D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Poppy Riddle" refreshedDate="45990.621988078703" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="324" xr:uid="{BE8D97D8-8858-4E4F-B159-AD67E1A7AF2D}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Sheet1"/>
   </cacheSource>
@@ -2814,12 +2851,13 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="error_classification" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
+      <sharedItems containsBlank="1" count="8">
         <s v="Inconsistent value representation"/>
-        <s v="semantic noise"/>
+        <s v="Information gain"/>
         <s v="Information loss"/>
         <m/>
         <s v="Missing information"/>
+        <s v="semantic noise"/>
         <s v="incorrect value"/>
         <s v="datatype noise"/>
       </sharedItems>
@@ -4305,7 +4343,7 @@
     <s v="1949, Commission on Human RightsDraft International Covenant on Human Rights: Fifth session"/>
     <b v="0"/>
     <n v="0.8"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.4103/ijohs.ijohs_8_21"/>
@@ -4313,7 +4351,7 @@
     <s v="Laser versus surgical: Different treatment modalities of mucocele: A case series"/>
     <b v="1"/>
     <n v="0.8"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1039/d5mh00046g"/>
@@ -4369,7 +4407,7 @@
     <s v="Ecospirituality and the Moralization of Nature"/>
     <b v="0"/>
     <n v="0.66666666666666663"/>
-    <x v="5"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="10.18795/gumusmaviatlas.681798"/>
@@ -4425,7 +4463,7 @@
     <s v="Observation of double &amp;lt;math display=&amp;quot;inline&amp;quot;&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;mi&amp;gt;J&amp;lt;/mi&amp;gt;&amp;lt;/mrow&amp;gt;&amp;lt;mo&amp;gt;/&amp;lt;/mo&amp;gt;&amp;lt;mi&amp;gt;ψ&amp;lt;/mi&amp;gt;&amp;lt;/math&amp;gt; meson production in &amp;lt;math display=&amp;quot;inline&amp;quot;&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;mi&amp;gt;p&amp;lt;/mi&amp;gt;&amp;lt;mi&amp;gt;Pb&amp;lt;/mi&amp;gt;&amp;lt;/mrow&amp;gt;&amp;lt;/math&amp;gt; collisions at &amp;lt;math display=&amp;quot;inline&amp;quot;&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;msqrt&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;msub&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;mi&amp;gt;s&amp;lt;/mi&amp;gt;&amp;lt;/mrow&amp;gt;&amp;lt;mrow&amp;gt;&amp;lt;mi&amp;gt;NN&amp;lt;/mi&amp;gt;&amp;lt;/…"/>
     <b v="0"/>
     <n v="0.6428571428571429"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.1093/jge/gxaf022"/>
@@ -4473,7 +4511,7 @@
     <s v="Part V New Financial Technology in Financial Markets and Infrastructure, 14 Fintech and Financial Markets Infrastructure—A Legal and Regulatory Perspective"/>
     <b v="0"/>
     <n v="0.5625"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.1093/molbev/msae108"/>
@@ -4487,9 +4525,9 @@
     <s v="10.22199/issn.0717-6279-6048"/>
     <s v="Higher order mKdV breathers"/>
     <s v="Higher order mKdV breathers: nonlinear stability"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.5"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.31260/repertmedcir.01217372.1235"/>
@@ -4497,7 +4535,7 @@
     <s v="Tratamiento endoscópico del Tratamiento endoscópico del divertículo de Zenker divertículo de Zenker"/>
     <b v="0"/>
     <n v="0.5"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.3847/2515-5172/ad7113"/>
@@ -4511,9 +4549,9 @@
     <s v="10.4103/srmjrds.srmjrds_46_22"/>
     <s v="Effects of platelet-rich fibrin in the surgical extraction of mandibular third molar"/>
     <s v="Effects of platelet-rich fibrin in the surgical extraction of mandibular third molar: A systematic review and meta-analysis"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.41666666666666669"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.15575/psy.v9i1.7571"/>
@@ -4537,7 +4575,7 @@
     <s v="Sürdürülebilirliğin Satın Alma Niyeti Üzerine Web of Science Veri Tabanı Aracılığıyla Bibliyometrik Bir Analiz"/>
     <b v="0"/>
     <n v="0.38461538461538458"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.1075/pbns.313.12luo"/>
@@ -4545,7 +4583,7 @@
     <s v="Chapter 12. Modified self-praise in social media"/>
     <b v="0"/>
     <n v="0.33333333333333331"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.1093/bioinformatics/btae516"/>
@@ -4567,9 +4605,9 @@
     <s v="10.1209/0295-5075/ada8d5"/>
     <s v="On the equation of motion in supersymmetric Yang-Mills plasma"/>
     <s v="On the equation of motion in N = 4 supersymmetric Yang-Mills plasma"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.33333333333333331"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1364/ol.551558"/>
@@ -4583,9 +4621,9 @@
     <s v="10.2174/0929866529666220905112156"/>
     <s v="Amplification of Amyloid Protein-induced Aggregation of the Eukaryotic_x000a_Ribosome"/>
     <s v="Amplification of Amyloid Protein-induced Aggregation of the Eukaryotic Ribosome"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.33333333333333331"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.33735/phimisci.2020.i.48"/>
@@ -4615,9 +4653,9 @@
     <s v="10.2174/0929867328666211214165814"/>
     <s v="A Novel Approach for Designing Electrochemical Aptamer-Based_x000a_Biosensor for Ultrasensitive Detection of Zearalenone as a Prevalent_x000a_Estrogenic Mycotoxin"/>
     <s v="A Novel Approach for Designing Electrochemical Aptamer-Based Biosensor for Ultrasensitive Detection of Zearalenone as a Prevalent Estrogenic Mycotoxin"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.30769230769230771"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1039/d2sc06436g"/>
@@ -4663,9 +4701,9 @@
     <s v="10.1039/d4sc06441k"/>
     <s v="Reassessing the role and lifetime of Q&lt;sub&gt;x&lt;/sub&gt; in the energy transfer dynamics of chlorophyll a"/>
     <s v="Reassessing the role and lifetime of Qx in the energy transfer dynamics of Chlorophyll a"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.25"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="10.1093/humrep/dead093.277"/>
@@ -4703,9 +4741,9 @@
     <s v="10.37741/t.71.4.2"/>
     <s v="Destination Choice,_x000a_Satisfaction, and Loyalty of Ski Tourists in the Indian Himalayas"/>
     <s v="Destination Choice, Satisfaction, and Loyalty of Ski Tourists in the Indian Himalayas"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.25"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1093/nop/npae008"/>
@@ -4831,17 +4869,17 @@
     <s v="10.1364/oe.541425"/>
     <s v="SNSPD-based detector system for NASA’s Deep Space Optical Communications project"/>
     <s v="An SNSPD-based detector system for NASA's Deep Space Optical Communications project"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.2"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1558/bar.18313"/>
     <s v="&amp;lt;i&amp;gt;Social Skins of the Head: Body Beliefs and Ritual in Ancient Mesoamerica and the Andes&amp;lt;/i&amp;gt; Edited by V. Tiesler and M. C. Lozada (2018)"/>
     <s v="Social Skins of the Head: Body Beliefs and Ritual in Ancient Mesoamerica and the Andes edited by V. Tiesler and M. C. Lozada (2018)"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1875"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="10.1039/d2en00837h"/>
@@ -4887,9 +4925,9 @@
     <s v="10.51220/jmr.v18i1.6"/>
     <s v="Repositioning Urban Agenda For Sustainable Development Goals In Jammu And_x000a_Kashmir"/>
     <s v="Repositioning Urban Agenda For Sustainable Development Goals In Jammu And Kashmir"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1818181818181818"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1002/chem.202402809"/>
@@ -4959,25 +4997,25 @@
     <s v="10.2174/1567202620666230303144323"/>
     <s v="Curcumin Alleviates Oxidative Stress, Neuroinflammation, and Promotes_x000a_Behavioral Recovery After Traumatic Brain Injury"/>
     <s v="Curcumin Alleviates Oxidative Stress, Neuroinflammation, and Promotes Behavioral Recovery After Traumatic Brain Injury"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.16666666666666671"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.21931/bj/2024.01.01.75"/>
     <s v="Evaluation of DNA damage through cytogenetic approach in smokers and vapers with and without_x000a_nicotine compared with control group"/>
     <s v="Evaluation of DNA damage through cytogenetic approach in smokers and vapers with and without nicotine compared with control group"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.16666666666666671"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.36937/ben.2024.4951"/>
     <s v="Development and Performance Evaluation of Push Type Manually Operated Hilling_x000a_Corn with Double Wheel Hoe"/>
     <s v="Development and Performance Evaluation of Push Type Manually Operated Hilling Corn with Double Wheel Hoe"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.16666666666666671"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1002/cbdv.202402361"/>
@@ -4999,9 +5037,9 @@
     <s v="10.5604/01.3001.0013.8156"/>
     <s v="SOLUTIONS ENSURING SAFETY DURING TRANSPORT_x000a_OF STATE VIPS BY MILITARY AIRFCRAFT (part 2)"/>
     <s v="SOLUTIONS ENSURING SAFETY DURING TRANSPORT OF STATE VIPS BY MILITARY AIRFCRAFT (part 2)"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.15384615384615391"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1002/ange.202424183"/>
@@ -5041,7 +5079,7 @@
     <s v="ЭФФЕКТИВНОСТЬ ПРИМЕНЕНИЯ КОРМОВОЙ ДОБАВКИ &quot;БЕТАКОРМ&quot; ПРИ КОКЦИДИОЗЕ ЦЫПЛЯТ-БРОЙЛЕРОВ Ильин Г.М., Рябцев П.С., Комарчев А.С."/>
     <b v="0"/>
     <n v="0.14285714285714279"/>
-    <x v="1"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="10.3389/fnut.2025.1551349"/>
@@ -5055,9 +5093,9 @@
     <s v="10.34091/ajss.13.2.04"/>
     <s v="The Effect of Explicit Knowledge Sharing on Human Resource Performance_x000a_Efficiency: Moderating Role of Human Capacity Development"/>
     <s v="The Effect of Explicit Knowledge Sharing on Human Resource Performance Efficiency: Moderating Role of Human Capacity Development"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.14285714285714279"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1002/nbm.5134"/>
@@ -5089,7 +5127,7 @@
     <s v="The Fourth Most Utility: - Compressed Air Engine"/>
     <b v="0"/>
     <n v="0.125"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.1002/jbm.a.37614"/>
@@ -5103,9 +5141,9 @@
     <s v="10.1039/d5ay00460h"/>
     <s v="A BODIPY-based fluorescent probe for rapid detection of NO in cells and zebrafish"/>
     <s v="BODIPY-based fluorescent probe for rapid detection of NO in cells and zebrafish"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="10.1093/bjs/znab430.230"/>
@@ -5129,7 +5167,7 @@
     <s v="Simulation Analysis &amp;amp; Image Processing of the Exhaust Silencing Chamber and Coil"/>
     <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.1158/1055-9965.epi-24-1398"/>
@@ -5145,15 +5183,15 @@
     <s v="Toxicologic Pathology Forum*: mRNA Vaccine Safety–Separating Fact From Fiction"/>
     <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.26656/fr.2017.5(6).125"/>
     <s v="Electronic nose to differentiate between several drying techniques for_x000a_Origanum syriacum leaves"/>
     <s v="Electronic nose to differentiate between several drying techniques for Origanum syriacum leaves"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.3828/index.2024.26"/>
@@ -5167,17 +5205,17 @@
     <s v="10.47836/mjms.17.3.05"/>
     <s v="Variable-order Implicit Fractional Differential Equations based on the_x000a_Kuratowski MNC Technique"/>
     <s v="Variable-order Implicit Fractional Differential Equations based on the Kuratowski MNC Technique"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.55529/jcfmbs.35.6.16"/>
     <s v="Assets Investment and Financial Performance of_x000a_Deposit Money Banks in Nigeria (2016-2021)"/>
     <s v="Assets Investment and Financial Performance of Deposit Money Banks in Nigeria (2016-2021)"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0.1111111111111111"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1111/neup.12938"/>
@@ -5201,7 +5239,7 @@
     <s v="Instrumental Non-Invasive Diagnostics of the Depth of Skin Burn:&amp;#x0D; Current Opportunities and Unsolved Problems"/>
     <b v="0"/>
     <n v="0.1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.1093/mnras/staf007"/>
@@ -5209,7 +5247,7 @@
     <s v="The XMM Cluster Survey: Automating the estimation of hydrostatic mass for large samples of galaxy clusters – I. Methodology, validation, &amp;amp; application to the SDSSRM-XCS sample"/>
     <b v="0"/>
     <n v="0.1"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.1093/humrep/deae108.1004"/>
@@ -5313,15 +5351,15 @@
     <s v="Reconstruction of global surface ocean &amp;amp;lt;i&amp;amp;gt;p&amp;amp;lt;/i&amp;amp;gt;CO&amp;amp;lt;sub&amp;amp;gt;2&amp;amp;lt;/sub&amp;amp;gt; using region-specific predictors based on a stepwise FFNN regression algorithm"/>
     <b v="0"/>
     <n v="7.6923076923076927E-2"/>
-    <x v="6"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="10.58818/ijems.v3i3.146"/>
     <s v="Effect of Emotional Maturity on Student Discipline in Participating in Activities at the College of Qur'an Sciences (STIQ) Amuntai"/>
     <s v="The Effect of Emotional Maturity on Student Discipline in Participating in Activities at the College of Qur'an Sciences (STIQ) Amuntai"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="7.6923076923076927E-2"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.61218/hadith.1541223"/>
@@ -5359,9 +5397,9 @@
     <s v="10.51220/jmr.v19-i2.10"/>
     <s v="A Comprehensive Review on Actinomycetes Distribution, Novel Bioactive Compounds_x000a_and Their Implementation in The Field of Agronomy And Medical"/>
     <s v="A Comprehensive Review on Actinomycetes Distribution, Novel Bioactive Compounds and Their Implementation in The Field of Agronomy And Medical"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="6.6666666666666666E-2"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1093/jambio/lxaf002"/>
@@ -5375,9 +5413,9 @@
     <s v="10.54151/27382559-2021.1b-292"/>
     <s v="ОБ ОДНОЙ ИЗ ПРИЧИН ТРУДНОСТЕЙ УСВОЕНИЯ ОМОНИМИИ ПРИ ОБУЧЕНИИ РУССКОМУ ЯЗЫКУ КАК НЕРОДНОМУ / ON ONE OF THE REASONS FOR THE DIFFICULTIES IN MASTERING_x000a_HOMONYMY WHILE TEACHING RUSSIAN AS A FOREIGN LANGUAGE"/>
     <s v="ОБ ОДНОЙ ИЗ ПРИЧИН ТРУДНОСТЕЙ УСВОЕНИЯ ОМОНИМИИ ПРИ ОБУЧЕНИИ РУССКОМУ ЯЗЫКУ КАК НЕРОДНОМУ / ON ONE OF THE REASONS FOR THE DIFFICULTIES IN MASTERING HOMONYMY WHILE TEACHING RUSSIAN AS A FOREIGN LANGUAGE"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="6.25E-2"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <s v="10.1002/ange.202414652"/>
@@ -5415,9 +5453,9 @@
     <s v="10.1115/1.4067013"/>
     <s v="Rolling Formability Optimization of Locking Bolt Based on a Double-Thread Structure Composed of Coaxial Single and Multiple Threads"/>
     <s v="Rolling Formability Optimization of Locking Bolt Based on Double-Thread Structure Composed of Coaxial Single and Multiple Threads"/>
-    <b v="1"/>
+    <b v="0"/>
     <n v="0"/>
-    <x v="3"/>
+    <x v="1"/>
   </r>
   <r>
     <m/>
@@ -5431,8 +5469,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6E3D8D78-8A13-1842-B1AE-ABB0BEB4CB29}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6E3D8D78-8A13-1842-B1AE-ABB0BEB4CB29}" name="PivotTable2" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -5440,14 +5478,15 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="8">
+      <items count="9">
+        <item x="7"/>
+        <item x="0"/>
         <item x="6"/>
-        <item x="0"/>
-        <item x="5"/>
         <item x="2"/>
         <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
         <item x="1"/>
-        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5455,7 +5494,7 @@
   <rowFields count="1">
     <field x="5"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x/>
     </i>
@@ -5477,6 +5516,9 @@
     <i>
       <x v="6"/>
     </i>
+    <i>
+      <x v="7"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -5487,6 +5529,11 @@
   <dataFields count="1">
     <dataField name="Count of error_classification" fld="5" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -5784,11 +5831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F307"/>
+    <sheetView topLeftCell="B296" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C329" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5841,7 +5887,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -5858,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>862</v>
+        <v>874</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6141,7 +6187,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>577</v>
       </c>
@@ -6381,7 +6427,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -6401,7 +6447,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -6421,7 +6467,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -6441,7 +6487,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -6461,7 +6507,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -6481,7 +6527,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -6501,7 +6547,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -6521,7 +6567,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -6541,7 +6587,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -6561,7 +6607,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -6581,7 +6627,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -6601,7 +6647,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -6621,7 +6667,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -6641,7 +6687,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -6661,7 +6707,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -6681,7 +6727,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -6701,7 +6747,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -6721,7 +6767,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -6741,7 +6787,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -6761,7 +6807,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -6781,7 +6827,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -6801,7 +6847,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -6821,7 +6867,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -6841,7 +6887,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -6861,7 +6907,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>99</v>
       </c>
@@ -6881,7 +6927,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -6901,7 +6947,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -6921,7 +6967,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>105</v>
       </c>
@@ -6941,7 +6987,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -6961,7 +7007,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -6981,7 +7027,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>111</v>
       </c>
@@ -7001,7 +7047,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>113</v>
       </c>
@@ -7021,7 +7067,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>118</v>
       </c>
@@ -7041,7 +7087,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -7061,7 +7107,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -7081,7 +7127,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -7101,7 +7147,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -7121,7 +7167,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -7141,7 +7187,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -7161,7 +7207,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -7181,7 +7227,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -7201,7 +7247,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -7221,7 +7267,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>144</v>
       </c>
@@ -7241,7 +7287,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -7261,7 +7307,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>280</v>
       </c>
@@ -7281,7 +7327,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>282</v>
       </c>
@@ -7301,7 +7347,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>332</v>
       </c>
@@ -7321,7 +7367,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>382</v>
       </c>
@@ -7341,7 +7387,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>384</v>
       </c>
@@ -7361,7 +7407,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>386</v>
       </c>
@@ -7381,7 +7427,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>421</v>
       </c>
@@ -7401,7 +7447,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>432</v>
       </c>
@@ -7421,7 +7467,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>434</v>
       </c>
@@ -7441,7 +7487,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>436</v>
       </c>
@@ -7461,7 +7507,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>438</v>
       </c>
@@ -7481,7 +7527,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>440</v>
       </c>
@@ -7501,7 +7547,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>442</v>
       </c>
@@ -7521,7 +7567,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>444</v>
       </c>
@@ -7541,7 +7587,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>446</v>
       </c>
@@ -7561,7 +7607,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>448</v>
       </c>
@@ -7581,7 +7627,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>450</v>
       </c>
@@ -7601,7 +7647,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>452</v>
       </c>
@@ -7621,7 +7667,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>454</v>
       </c>
@@ -7641,7 +7687,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>456</v>
       </c>
@@ -7661,7 +7707,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>458</v>
       </c>
@@ -7681,7 +7727,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>460</v>
       </c>
@@ -7701,7 +7747,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>462</v>
       </c>
@@ -7721,7 +7767,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>464</v>
       </c>
@@ -7741,7 +7787,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>466</v>
       </c>
@@ -7761,7 +7807,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>468</v>
       </c>
@@ -7781,7 +7827,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>470</v>
       </c>
@@ -7801,7 +7847,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>472</v>
       </c>
@@ -7821,7 +7867,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>474</v>
       </c>
@@ -7841,7 +7887,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>476</v>
       </c>
@@ -7861,7 +7907,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>478</v>
       </c>
@@ -7881,7 +7927,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>480</v>
       </c>
@@ -7901,7 +7947,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>494</v>
       </c>
@@ -7921,7 +7967,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>496</v>
       </c>
@@ -7941,7 +7987,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>498</v>
       </c>
@@ -7961,7 +8007,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>500</v>
       </c>
@@ -7981,7 +8027,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>508</v>
       </c>
@@ -8001,7 +8047,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>510</v>
       </c>
@@ -8021,7 +8067,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>512</v>
       </c>
@@ -8041,7 +8087,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>514</v>
       </c>
@@ -8061,7 +8107,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>519</v>
       </c>
@@ -8081,7 +8127,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>533</v>
       </c>
@@ -8101,7 +8147,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>535</v>
       </c>
@@ -8121,7 +8167,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>573</v>
       </c>
@@ -8141,7 +8187,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>575</v>
       </c>
@@ -8161,7 +8207,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>649</v>
       </c>
@@ -8181,7 +8227,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>651</v>
       </c>
@@ -8201,7 +8247,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>653</v>
       </c>
@@ -8221,7 +8267,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>655</v>
       </c>
@@ -8241,7 +8287,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>657</v>
       </c>
@@ -8261,7 +8307,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>659</v>
       </c>
@@ -8281,7 +8327,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>676</v>
       </c>
@@ -8301,7 +8347,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>678</v>
       </c>
@@ -8321,7 +8367,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>707</v>
       </c>
@@ -8341,7 +8387,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>709</v>
       </c>
@@ -8361,7 +8407,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>747</v>
       </c>
@@ -8381,7 +8427,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>749</v>
       </c>
@@ -8401,7 +8447,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>760</v>
       </c>
@@ -8421,7 +8467,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>771</v>
       </c>
@@ -8441,7 +8487,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>773</v>
       </c>
@@ -8461,7 +8507,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>775</v>
       </c>
@@ -8481,7 +8527,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>819</v>
       </c>
@@ -8501,7 +8547,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>726</v>
       </c>
@@ -8518,7 +8564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>824</v>
       </c>
@@ -8538,7 +8584,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>826</v>
       </c>
@@ -8558,7 +8604,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>852</v>
       </c>
@@ -8578,7 +8624,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>854</v>
       </c>
@@ -8598,7 +8644,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>218</v>
       </c>
@@ -8618,7 +8664,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>586</v>
       </c>
@@ -8638,7 +8684,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>588</v>
       </c>
@@ -8818,7 +8864,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>502</v>
       </c>
@@ -9078,7 +9124,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>173</v>
       </c>
@@ -9155,7 +9201,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>20</v>
       </c>
@@ -9192,7 +9238,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>191</v>
       </c>
@@ -9209,7 +9255,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>485</v>
       </c>
@@ -9266,7 +9312,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>167</v>
       </c>
@@ -9286,7 +9332,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>355</v>
       </c>
@@ -9303,7 +9349,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>527</v>
       </c>
@@ -9320,7 +9366,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>616</v>
       </c>
@@ -9337,7 +9383,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>164</v>
       </c>
@@ -9374,7 +9420,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>239</v>
       </c>
@@ -9391,7 +9437,7 @@
         <v>0.84615384615384615</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>373</v>
       </c>
@@ -9408,7 +9454,7 @@
         <v>0.84615384615384615</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>185</v>
       </c>
@@ -9425,7 +9471,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>269</v>
       </c>
@@ -9442,7 +9488,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>284</v>
       </c>
@@ -9462,7 +9508,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>762</v>
       </c>
@@ -9478,8 +9524,11 @@
       <c r="E186">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F186" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -9496,7 +9545,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>308</v>
       </c>
@@ -9513,7 +9562,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>242</v>
       </c>
@@ -9530,7 +9579,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>765</v>
       </c>
@@ -9547,7 +9596,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>126</v>
       </c>
@@ -9564,7 +9613,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>158</v>
       </c>
@@ -9581,7 +9630,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>426</v>
       </c>
@@ -9641,7 +9690,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>418</v>
       </c>
@@ -9658,7 +9707,7 @@
         <v>0.65217391304347827</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>152</v>
       </c>
@@ -9695,7 +9744,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>589</v>
       </c>
@@ -9715,7 +9764,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>329</v>
       </c>
@@ -9735,7 +9784,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>275</v>
       </c>
@@ -9752,7 +9801,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>54</v>
       </c>
@@ -9769,7 +9818,7 @@
         <v>0.61538461538461542</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>200</v>
       </c>
@@ -9786,10 +9835,10 @@
         <v>0.61538461538461542</v>
       </c>
       <c r="F203" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>337</v>
       </c>
@@ -9806,7 +9855,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>415</v>
       </c>
@@ -9823,7 +9872,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>287</v>
       </c>
@@ -9843,7 +9892,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>302</v>
       </c>
@@ -9860,7 +9909,7 @@
         <v>0.53846153846153844</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>610</v>
       </c>
@@ -9871,13 +9920,16 @@
         <v>612</v>
       </c>
       <c r="D208" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E208">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F208" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>646</v>
       </c>
@@ -9897,7 +9949,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>744</v>
       </c>
@@ -9914,7 +9966,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>768</v>
       </c>
@@ -9925,13 +9977,16 @@
         <v>770</v>
       </c>
       <c r="D211" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E211">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F211" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>537</v>
       </c>
@@ -9951,7 +10006,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>521</v>
       </c>
@@ -9968,7 +10023,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>634</v>
       </c>
@@ -9988,7 +10043,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>215</v>
       </c>
@@ -10008,7 +10063,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>227</v>
       </c>
@@ -10025,7 +10080,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>263</v>
       </c>
@@ -10042,7 +10097,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>482</v>
       </c>
@@ -10053,13 +10108,16 @@
         <v>484</v>
       </c>
       <c r="D218" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E218">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F218" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>516</v>
       </c>
@@ -10076,7 +10134,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>592</v>
       </c>
@@ -10087,13 +10145,16 @@
         <v>594</v>
       </c>
       <c r="D220" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E220">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F220" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>683</v>
       </c>
@@ -10110,7 +10171,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>403</v>
       </c>
@@ -10127,7 +10188,7 @@
         <v>0.31578947368421051</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>732</v>
       </c>
@@ -10144,7 +10205,7 @@
         <v>0.31578947368421051</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>595</v>
       </c>
@@ -10155,13 +10216,16 @@
         <v>597</v>
       </c>
       <c r="D224" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E224">
         <v>0.30769230769230771</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F224" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>149</v>
       </c>
@@ -10178,7 +10242,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>221</v>
       </c>
@@ -10195,7 +10259,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>170</v>
       </c>
@@ -10212,7 +10276,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>42</v>
       </c>
@@ -10229,7 +10293,7 @@
         <v>0.26315789473684209</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>11</v>
       </c>
@@ -10246,7 +10310,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>176</v>
       </c>
@@ -10257,13 +10321,16 @@
         <v>178</v>
       </c>
       <c r="D230" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E230">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F230" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>254</v>
       </c>
@@ -10280,7 +10347,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>326</v>
       </c>
@@ -10297,7 +10364,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>367</v>
       </c>
@@ -10314,7 +10381,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>429</v>
       </c>
@@ -10331,7 +10398,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>735</v>
       </c>
@@ -10342,13 +10409,16 @@
         <v>737</v>
       </c>
       <c r="D235" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E235">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F235" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>305</v>
       </c>
@@ -10365,7 +10435,7 @@
         <v>0.23076923076923081</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>379</v>
       </c>
@@ -10382,7 +10452,7 @@
         <v>0.23076923076923081</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>257</v>
       </c>
@@ -10399,7 +10469,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>334</v>
       </c>
@@ -10416,7 +10486,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>346</v>
       </c>
@@ -10433,7 +10503,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>397</v>
       </c>
@@ -10450,7 +10520,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>488</v>
       </c>
@@ -10467,7 +10537,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>133</v>
       </c>
@@ -10484,7 +10554,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>209</v>
       </c>
@@ -10501,7 +10571,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>248</v>
       </c>
@@ -10518,7 +10588,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>314</v>
       </c>
@@ -10535,7 +10605,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>320</v>
       </c>
@@ -10552,7 +10622,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>343</v>
       </c>
@@ -10569,7 +10639,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>409</v>
       </c>
@@ -10586,7 +10656,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>491</v>
       </c>
@@ -10603,7 +10673,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>505</v>
       </c>
@@ -10614,13 +10684,16 @@
         <v>507</v>
       </c>
       <c r="D251" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E251">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F251" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>540</v>
       </c>
@@ -10631,13 +10704,16 @@
         <v>542</v>
       </c>
       <c r="D252" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E252">
         <v>0.1875</v>
       </c>
-    </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F252" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>146</v>
       </c>
@@ -10654,7 +10730,7 @@
         <v>0.1818181818181818</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>245</v>
       </c>
@@ -10671,7 +10747,7 @@
         <v>0.1818181818181818</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>311</v>
       </c>
@@ -10688,7 +10764,7 @@
         <v>0.1818181818181818</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>394</v>
       </c>
@@ -10705,7 +10781,7 @@
         <v>0.1818181818181818</v>
       </c>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>692</v>
       </c>
@@ -10725,7 +10801,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>789</v>
       </c>
@@ -10736,13 +10812,16 @@
         <v>791</v>
       </c>
       <c r="D258" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E258">
         <v>0.1818181818181818</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F258" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>17</v>
       </c>
@@ -10759,7 +10838,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>48</v>
       </c>
@@ -10776,7 +10855,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>230</v>
       </c>
@@ -10793,7 +10872,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>233</v>
       </c>
@@ -10810,7 +10889,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>251</v>
       </c>
@@ -10827,7 +10906,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>290</v>
       </c>
@@ -10844,7 +10923,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>317</v>
       </c>
@@ -10861,7 +10940,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>364</v>
       </c>
@@ -10878,7 +10957,7 @@
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>598</v>
       </c>
@@ -10889,13 +10968,16 @@
         <v>600</v>
       </c>
       <c r="D267" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E267">
         <v>0.16666666666666671</v>
       </c>
-    </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F267" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>607</v>
       </c>
@@ -10906,13 +10988,16 @@
         <v>609</v>
       </c>
       <c r="D268" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E268">
         <v>0.16666666666666671</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F268" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>729</v>
       </c>
@@ -10923,13 +11008,16 @@
         <v>731</v>
       </c>
       <c r="D269" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E269">
         <v>0.16666666666666671</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F269" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>14</v>
       </c>
@@ -10946,7 +11034,7 @@
         <v>0.15384615384615391</v>
       </c>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>197</v>
       </c>
@@ -10963,7 +11051,7 @@
         <v>0.15384615384615391</v>
       </c>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>834</v>
       </c>
@@ -10974,13 +11062,16 @@
         <v>836</v>
       </c>
       <c r="D272" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E272">
         <v>0.15384615384615391</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F272" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>8</v>
       </c>
@@ -10997,7 +11088,7 @@
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>45</v>
       </c>
@@ -11014,7 +11105,7 @@
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>203</v>
       </c>
@@ -11031,7 +11122,7 @@
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>296</v>
       </c>
@@ -11048,7 +11139,7 @@
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>686</v>
       </c>
@@ -11068,7 +11159,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>689</v>
       </c>
@@ -11085,7 +11176,7 @@
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>701</v>
       </c>
@@ -11096,13 +11187,16 @@
         <v>703</v>
       </c>
       <c r="D279" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E279">
         <v>0.14285714285714279</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F279" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>51</v>
       </c>
@@ -11119,7 +11213,7 @@
         <v>0.1333333333333333</v>
       </c>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>212</v>
       </c>
@@ -11136,7 +11230,7 @@
         <v>0.1333333333333333</v>
       </c>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>388</v>
       </c>
@@ -11153,7 +11247,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>720</v>
       </c>
@@ -11173,7 +11267,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>39</v>
       </c>
@@ -11190,7 +11284,7 @@
         <v>0.1176470588235294</v>
       </c>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>188</v>
       </c>
@@ -11201,13 +11295,16 @@
         <v>190</v>
       </c>
       <c r="D285" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E285">
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F285" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>236</v>
       </c>
@@ -11224,7 +11321,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>323</v>
       </c>
@@ -11241,7 +11338,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>370</v>
       </c>
@@ -11261,7 +11358,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>412</v>
       </c>
@@ -11278,7 +11375,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>423</v>
       </c>
@@ -11298,7 +11395,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>625</v>
       </c>
@@ -11309,13 +11406,16 @@
         <v>627</v>
       </c>
       <c r="D291" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E291">
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F291" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>741</v>
       </c>
@@ -11332,7 +11432,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>786</v>
       </c>
@@ -11343,13 +11443,16 @@
         <v>788</v>
       </c>
       <c r="D293" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E293">
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F293" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>821</v>
       </c>
@@ -11360,13 +11463,16 @@
         <v>823</v>
       </c>
       <c r="D294" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E294">
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F294" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>352</v>
       </c>
@@ -11383,7 +11489,7 @@
         <v>0.10526315789473679</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>661</v>
       </c>
@@ -11403,7 +11509,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>564</v>
       </c>
@@ -11423,7 +11529,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>299</v>
       </c>
@@ -11443,7 +11549,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>260</v>
       </c>
@@ -11460,7 +11566,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>161</v>
       </c>
@@ -11477,7 +11583,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>206</v>
       </c>
@@ -11497,7 +11603,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>182</v>
       </c>
@@ -11517,7 +11623,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>272</v>
       </c>
@@ -11534,7 +11640,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>36</v>
       </c>
@@ -11571,7 +11677,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>224</v>
       </c>
@@ -11611,7 +11717,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>695</v>
       </c>
@@ -11628,7 +11734,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>406</v>
       </c>
@@ -11648,7 +11754,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>400</v>
       </c>
@@ -11668,7 +11774,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>804</v>
       </c>
@@ -11688,7 +11794,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>840</v>
       </c>
@@ -11699,13 +11805,16 @@
         <v>842</v>
       </c>
       <c r="D312" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E312">
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F312" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>846</v>
       </c>
@@ -11722,7 +11831,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>293</v>
       </c>
@@ -11739,7 +11848,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>391</v>
       </c>
@@ -11756,7 +11865,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>340</v>
       </c>
@@ -11773,7 +11882,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>792</v>
       </c>
@@ -11784,13 +11893,16 @@
         <v>794</v>
       </c>
       <c r="D317" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E317">
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F317" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>266</v>
       </c>
@@ -11807,7 +11919,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>816</v>
       </c>
@@ -11818,13 +11930,16 @@
         <v>818</v>
       </c>
       <c r="D319" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E319">
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F319" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>5</v>
       </c>
@@ -11841,7 +11956,7 @@
         <v>5.8823529411764712E-2</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>757</v>
       </c>
@@ -11858,7 +11973,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>155</v>
       </c>
@@ -11875,7 +11990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>179</v>
       </c>
@@ -11892,7 +12007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>358</v>
       </c>
@@ -11903,25 +12018,16 @@
         <v>360</v>
       </c>
       <c r="D324" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E324">
         <v>0</v>
       </c>
+      <c r="F324" t="s">
+        <v>875</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F324" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Inconsistent value representation"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F311">
     <sortCondition descending="1" ref="E2:E324"/>
     <sortCondition ref="C2:C324"/>
@@ -11932,23 +12038,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D55A398-1037-5740-9F55-79BCF1AB99FE}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>869</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>872</v>
       </c>
     </row>
@@ -11956,7 +12062,7 @@
       <c r="A2" s="4" t="s">
         <v>864</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>7</v>
       </c>
     </row>
@@ -11964,7 +12070,7 @@
       <c r="A3" s="4" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>58</v>
       </c>
     </row>
@@ -11972,7 +12078,7 @@
       <c r="A4" s="4" t="s">
         <v>865</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
     </row>
@@ -11980,15 +12086,15 @@
       <c r="A5" s="4" t="s">
         <v>866</v>
       </c>
-      <c r="B5" s="5">
-        <v>123</v>
+      <c r="B5" s="6">
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>867</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
     </row>
@@ -11996,122 +12102,191 @@
       <c r="A7" s="4" t="s">
         <v>862</v>
       </c>
-      <c r="B7" s="5">
-        <v>8</v>
+      <c r="B7" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="B9" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>871</v>
       </c>
-      <c r="B9" s="5">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B10" s="6">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>877</v>
+      </c>
+      <c r="C15">
+        <v>9988</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>869</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>873</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C18" s="8" t="s">
+        <v>879</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>866</v>
+      </c>
+      <c r="B19">
+        <v>126</v>
+      </c>
+      <c r="C19" s="5">
+        <f>B19/$B$26</f>
+        <v>0.56502242152466364</v>
+      </c>
+      <c r="D19" s="5">
+        <f>B19/$C$15</f>
+        <v>1.2615138165798959E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>863</v>
+      </c>
+      <c r="B20">
+        <v>58</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" ref="C20:C26" si="0">B20/$B$26</f>
+        <v>0.26008968609865468</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" ref="D20:D26" si="1">B20/$C$15</f>
+        <v>5.8069683620344415E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>874</v>
       </c>
-      <c r="C16">
-        <v>9988</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>866</v>
-      </c>
-      <c r="B17">
-        <v>123</v>
-      </c>
-      <c r="C17" s="6">
-        <f>B17/$C$16</f>
-        <v>1.2314777733279936E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>863</v>
-      </c>
-      <c r="B18">
-        <v>58</v>
-      </c>
-      <c r="C18" s="6">
-        <f t="shared" ref="C18:C23" si="0">B18/$C$16</f>
-        <v>5.8069683620344415E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1031390134529148</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="1"/>
+        <v>2.3027633159791749E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>862</v>
       </c>
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5">
         <f t="shared" si="0"/>
-        <v>8.0096115338406087E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+        <v>2.6905829596412557E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="1"/>
+        <v>6.0072086503804565E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>864</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>7</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C23" s="5">
         <f t="shared" si="0"/>
+        <v>3.1390134529147982E-2</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="1"/>
         <v>7.0084100921105326E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>867</v>
       </c>
-      <c r="B21">
+      <c r="B24">
         <v>2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C24" s="5">
         <f t="shared" si="0"/>
+        <v>8.9686098654708519E-3</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="1"/>
         <v>2.0024028834601522E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>865</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
         <f t="shared" si="0"/>
+        <v>4.4843049327354259E-3</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="1"/>
         <v>1.0012014417300761E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>871</v>
       </c>
-      <c r="B23">
-        <v>199</v>
-      </c>
-      <c r="C23" s="6">
+      <c r="B26">
+        <v>223</v>
+      </c>
+      <c r="C26" s="5">
         <f t="shared" si="0"/>
-        <v>1.9923908690428514E-2</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="1"/>
+        <v>2.2326792150580695E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:B23">
-    <sortCondition descending="1" ref="B16:B23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:B26">
+    <sortCondition descending="1" ref="B18:B26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>